<commit_message>
Corrected a typographical error
</commit_message>
<xml_diff>
--- a/data-sync-excel/src/main/resources/Chemical treatment process .xlsx
+++ b/data-sync-excel/src/main/resources/Chemical treatment process .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamilchmiel/Desktop/Projects/DataSyncExcel/data-sync-excel/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5714624E-B53E-FA43-B30A-9E1AC8E79512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27886D9-4740-4C4E-91CB-38591FB41F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1000" windowWidth="27840" windowHeight="15300" xr2:uid="{69F6C0AC-BE0E-F54A-B367-7B3C8B8B754F}"/>
   </bookViews>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD01D58B-D7C5-1F45-86FF-A3CCF38FBF36}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +761,7 @@
         <v>4.5</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G3:G8" si="11">(F4*100)/D4</f>
+        <f t="shared" ref="G4:G8" si="11">(F4*100)/D4</f>
         <v>15.254237288135593</v>
       </c>
       <c r="H4" t="s">

</xml_diff>

<commit_message>
corrections and bug fixing (added correct file url, cases names in ExcelFileReader are updatet to be consistenc with excel file)
</commit_message>
<xml_diff>
--- a/data-sync-excel/src/main/resources/Chemical treatment process .xlsx
+++ b/data-sync-excel/src/main/resources/Chemical treatment process .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamilchmiel/Desktop/Projects/DataSyncExcel/data-sync-excel/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C34A09-221C-2C40-9959-35DDCBC9D7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C39C9-89E9-454F-A8BB-B84AE82FA939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1000" windowWidth="27840" windowHeight="15300" xr2:uid="{69F6C0AC-BE0E-F54A-B367-7B3C8B8B754F}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t xml:space="preserve">Prepared by </t>
   </si>
   <si>
-    <t>Recived back</t>
-  </si>
-  <si>
     <t xml:space="preserve">Result of the tested sample </t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Sale price 100% marge</t>
+  </si>
+  <si>
+    <t>Received back</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,49 +529,49 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#11 added mapping json file
</commit_message>
<xml_diff>
--- a/data-sync-excel/src/main/resources/Chemical treatment process .xlsx
+++ b/data-sync-excel/src/main/resources/Chemical treatment process .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamilchmiel/Desktop/Projects/DataSyncExcel/data-sync-excel/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C39C9-89E9-454F-A8BB-B84AE82FA939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99926D3C-E168-7D43-99E6-FDC7DCDC6A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1000" windowWidth="27840" windowHeight="15300" xr2:uid="{69F6C0AC-BE0E-F54A-B367-7B3C8B8B754F}"/>
   </bookViews>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD01D58B-D7C5-1F45-86FF-A3CCF38FBF36}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>